<commit_message>
PrintCalendar compete up to printing the month body
</commit_message>
<xml_diff>
--- a/PrintCalendar/First Day of Year.xlsx
+++ b/PrintCalendar/First Day of Year.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="24780" windowHeight="13170"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="16935" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,6 +815,21 @@
       <c r="H10">
         <v>37</v>
       </c>
+      <c r="J10">
+        <v>2012</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10" si="3">MOD(J10, $H$20)</f>
+        <v>80</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10" si="4">MOD(K10,$H$2)</f>
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="5">INT(K10/$H$2)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
@@ -934,7 +949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="2">
         <v>5</v>
@@ -958,7 +973,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -967,7 +982,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>6</v>
       </c>
@@ -993,7 +1008,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="2">
         <v>6</v>
@@ -1015,6 +1030,58 @@
       </c>
       <c r="H20">
         <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>60</v>
+      </c>
+      <c r="H26">
+        <v>121</v>
+      </c>
+      <c r="I26">
+        <v>120</v>
+      </c>
+      <c r="J26">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <f>MOD(G26,7)</f>
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <f>MOD(H26,7)</f>
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <f>MOD(I26,7)</f>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <f>MOD(J26,7)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>31</v>
+      </c>
+      <c r="F33">
+        <v>28</v>
+      </c>
+      <c r="G33">
+        <v>31</v>
+      </c>
+      <c r="H33">
+        <v>30</v>
+      </c>
+      <c r="I33">
+        <v>31</v>
+      </c>
+      <c r="J33">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>